<commit_message>
feat: create and setup login prefab and database scripts
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/tsv_UI_Defaults.xlsx
+++ b/Assets/StreamingAssets/tsv_UI_Defaults.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\draik\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Unity Project\metho_misession_MarcSeb\Assets\StreamingAssets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF331926-2C82-46E8-A0C9-A9F12F4780CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D62B464B-F7B8-4900-838A-3E937F448261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="87">
   <si>
     <t>Notes</t>
   </si>
@@ -194,6 +194,93 @@
   </si>
   <si>
     <t>Main menu</t>
+  </si>
+  <si>
+    <t>btn validate</t>
+  </si>
+  <si>
+    <t>Validate</t>
+  </si>
+  <si>
+    <t>Valider</t>
+  </si>
+  <si>
+    <t>UI Login</t>
+  </si>
+  <si>
+    <t>tmp login</t>
+  </si>
+  <si>
+    <t>UI Sign up</t>
+  </si>
+  <si>
+    <t>Sign up</t>
+  </si>
+  <si>
+    <t>Log in</t>
+  </si>
+  <si>
+    <t>Connexion</t>
+  </si>
+  <si>
+    <t>Inscription</t>
+  </si>
+  <si>
+    <t>tmp signup</t>
+  </si>
+  <si>
+    <t>UI email</t>
+  </si>
+  <si>
+    <t>tmp email</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>UI password</t>
+  </si>
+  <si>
+    <t>tmp password</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Mot de passe</t>
+  </si>
+  <si>
+    <t>UI confirm email</t>
+  </si>
+  <si>
+    <t>tmp confirm email</t>
+  </si>
+  <si>
+    <t>To gain access to ZombieSurvivor's features, please verify your e-mail address.</t>
+  </si>
+  <si>
+    <t>Pour accéder aux fonctionnalités de ZombieSurvivor, veuillez vérifier votre adresse e-mail.</t>
+  </si>
+  <si>
+    <t>tmp valid key</t>
+  </si>
+  <si>
+    <t>UI Game key</t>
+  </si>
+  <si>
+    <t>tmp invalid key</t>
+  </si>
+  <si>
+    <t>Invalid Key!</t>
+  </si>
+  <si>
+    <t>Clé invalide!</t>
+  </si>
+  <si>
+    <t>Valid key!</t>
+  </si>
+  <si>
+    <t>Clé valide!</t>
   </si>
 </sst>
 </file>
@@ -704,15 +791,20 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1068,19 +1160,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="17.88671875" customWidth="1"/>
+    <col min="1" max="1" width="19.21875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.21875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="17.88671875" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -1100,276 +1193,404 @@
       <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B14" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C15" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D15" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B16" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C16" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D16" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B17" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C17" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D17" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B18" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C18" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D18" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B19" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C19" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D19" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B20" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C20" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D20" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B21" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C21" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D21" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B22" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C22" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D22" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B23" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C23" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D23" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B24" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C24" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D24" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B25" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C25" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D25" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B26" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C26" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D26" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: add localization texts for login validation
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/tsv_UI_Defaults.xlsx
+++ b/Assets/StreamingAssets/tsv_UI_Defaults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Unity Project\metho_misession_MarcSeb\Assets\StreamingAssets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D62B464B-F7B8-4900-838A-3E937F448261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A8130F9-72A7-431B-BCBE-F3BB81E2B9CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="94">
   <si>
     <t>Notes</t>
   </si>
@@ -281,6 +281,27 @@
   </si>
   <si>
     <t>Clé valide!</t>
+  </si>
+  <si>
+    <t>UI Login feedback</t>
+  </si>
+  <si>
+    <t>tmp valid login</t>
+  </si>
+  <si>
+    <t>Connexion réussie!</t>
+  </si>
+  <si>
+    <t>tmp invalid login</t>
+  </si>
+  <si>
+    <t>Successfully logged in!</t>
+  </si>
+  <si>
+    <t>Invalid logins!</t>
+  </si>
+  <si>
+    <t>Informations de connexion invalides!</t>
   </si>
 </sst>
 </file>
@@ -1160,10 +1181,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1354,96 +1375,96 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>13</v>
+        <v>81</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>12</v>
+        <v>86</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>15</v>
+        <v>81</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>14</v>
+        <v>82</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>39</v>
+        <v>83</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
@@ -1453,13 +1474,13 @@
         <v>9</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
@@ -1469,13 +1490,13 @@
         <v>9</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
@@ -1485,13 +1506,13 @@
         <v>9</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
@@ -1501,45 +1522,45 @@
         <v>9</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
@@ -1549,48 +1570,80 @@
         <v>22</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
refactor: merge prefabs for login and signup into one
Also created a prefab for the promo code
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/tsv_UI_Defaults.xlsx
+++ b/Assets/StreamingAssets/tsv_UI_Defaults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Unity Project\metho_misession_MarcSeb\Assets\StreamingAssets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A8130F9-72A7-431B-BCBE-F3BB81E2B9CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1285C80E-C69D-4963-92CE-26E741254593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="98">
   <si>
     <t>Notes</t>
   </si>
@@ -302,6 +302,18 @@
   </si>
   <si>
     <t>Informations de connexion invalides!</t>
+  </si>
+  <si>
+    <t>UI Promo code</t>
+  </si>
+  <si>
+    <t>tmp promo code</t>
+  </si>
+  <si>
+    <t>Promo Code</t>
+  </si>
+  <si>
+    <t>Code Promotionnel</t>
   </si>
 </sst>
 </file>
@@ -1181,10 +1193,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1645,6 +1657,22 @@
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
     </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
feat: create and implement logic for visual cues on login & signin
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/tsv_UI_Defaults.xlsx
+++ b/Assets/StreamingAssets/tsv_UI_Defaults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Unity Project\metho_misession_MarcSeb\Assets\StreamingAssets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1285C80E-C69D-4963-92CE-26E741254593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C720391B-1C83-4982-AA93-45D5ECF4E6A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="105">
   <si>
     <t>Notes</t>
   </si>
@@ -314,6 +314,27 @@
   </si>
   <si>
     <t>Code Promotionnel</t>
+  </si>
+  <si>
+    <t>UI Signup feedback</t>
+  </si>
+  <si>
+    <t>tmp valid signup</t>
+  </si>
+  <si>
+    <t>tmp invalid signup</t>
+  </si>
+  <si>
+    <t>Votre compte a été créé!</t>
+  </si>
+  <si>
+    <t>Account could not be created.</t>
+  </si>
+  <si>
+    <t>Échec de la création du compte.</t>
+  </si>
+  <si>
+    <t>Account created!</t>
   </si>
 </sst>
 </file>
@@ -1193,10 +1214,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1419,96 +1440,96 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>81</v>
+        <v>98</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>80</v>
+        <v>99</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>85</v>
+        <v>104</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>81</v>
+        <v>98</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>83</v>
+        <v>102</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>84</v>
+        <v>103</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>13</v>
+        <v>81</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>12</v>
+        <v>86</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>15</v>
+        <v>81</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>14</v>
+        <v>82</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>39</v>
+        <v>83</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
@@ -1518,13 +1539,13 @@
         <v>9</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
@@ -1534,13 +1555,13 @@
         <v>9</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
@@ -1550,13 +1571,13 @@
         <v>9</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
@@ -1566,45 +1587,45 @@
         <v>9</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
@@ -1614,64 +1635,96 @@
         <v>22</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>94</v>
+        <v>30</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>95</v>
+        <v>31</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>96</v>
+        <v>49</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>97</v>
+        <v>49</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: add localization and audio cues
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/tsv_UI_Defaults.xlsx
+++ b/Assets/StreamingAssets/tsv_UI_Defaults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Unity Project\metho_misession_MarcSeb\Assets\StreamingAssets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C720391B-1C83-4982-AA93-45D5ECF4E6A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F026C86C-EB4A-4267-A899-B1F469DF7A13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="108">
   <si>
     <t>Notes</t>
   </si>
@@ -335,6 +335,15 @@
   </si>
   <si>
     <t>Account created!</t>
+  </si>
+  <si>
+    <t>btn logout</t>
+  </si>
+  <si>
+    <t>Log out</t>
+  </si>
+  <si>
+    <t>Déconnexion</t>
   </si>
 </sst>
 </file>
@@ -1214,10 +1223,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1283,13 +1292,13 @@
         <v>8</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>4</v>
+        <v>105</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>56</v>
+        <v>106</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>52</v>
+        <v>107</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
@@ -1299,13 +1308,13 @@
         <v>8</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
@@ -1315,173 +1324,173 @@
         <v>8</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>58</v>
+        <v>7</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>87</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>98</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>81</v>
+        <v>98</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>85</v>
+        <v>102</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>86</v>
+        <v>103</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
@@ -1491,61 +1500,61 @@
         <v>81</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>13</v>
+        <v>81</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>10</v>
+        <v>82</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>11</v>
+        <v>83</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>12</v>
+        <v>84</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
@@ -1555,13 +1564,13 @@
         <v>9</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
@@ -1571,13 +1580,13 @@
         <v>9</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
@@ -1587,13 +1596,13 @@
         <v>9</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
@@ -1603,13 +1612,13 @@
         <v>9</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
@@ -1619,29 +1628,29 @@
         <v>9</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
@@ -1651,13 +1660,13 @@
         <v>22</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
@@ -1667,29 +1676,29 @@
         <v>22</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
@@ -1699,32 +1708,48 @@
         <v>30</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
-        <v>94</v>
+        <v>30</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>95</v>
+        <v>32</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>96</v>
+        <v>48</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>97</v>
+        <v>47</v>
       </c>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: add noto font to project to support chinese characters
Note: Need to finish setting up prefabs
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/tsv_UI_Defaults.xlsx
+++ b/Assets/StreamingAssets/tsv_UI_Defaults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Unity Project\metho_misession_MarcSeb\Assets\StreamingAssets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F026C86C-EB4A-4267-A899-B1F469DF7A13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6352DA21-88EE-43F1-B0E2-8DA84E512FE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tsv_UI_Defaults" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="219">
   <si>
     <t>Notes</t>
   </si>
@@ -256,12 +256,6 @@
     <t>tmp confirm email</t>
   </si>
   <si>
-    <t>To gain access to ZombieSurvivor's features, please verify your e-mail address.</t>
-  </si>
-  <si>
-    <t>Pour accéder aux fonctionnalités de ZombieSurvivor, veuillez vérifier votre adresse e-mail.</t>
-  </si>
-  <si>
     <t>tmp valid key</t>
   </si>
   <si>
@@ -298,12 +292,6 @@
     <t>Successfully logged in!</t>
   </si>
   <si>
-    <t>Invalid logins!</t>
-  </si>
-  <si>
-    <t>Informations de connexion invalides!</t>
-  </si>
-  <si>
     <t>UI Promo code</t>
   </si>
   <si>
@@ -344,6 +332,351 @@
   </si>
   <si>
     <t>Déconnexion</t>
+  </si>
+  <si>
+    <t>tmp invalid email format</t>
+  </si>
+  <si>
+    <t>tmp invalid password</t>
+  </si>
+  <si>
+    <t>The email format was invalid.</t>
+  </si>
+  <si>
+    <t>Le format d'email utilisé est invalide.</t>
+  </si>
+  <si>
+    <t>Le mot de passe utilisé est invalide.</t>
+  </si>
+  <si>
+    <t>The password was invalid.</t>
+  </si>
+  <si>
+    <t>Échec de la connexion.</t>
+  </si>
+  <si>
+    <t>Login has failed.</t>
+  </si>
+  <si>
+    <t>tmp email already used</t>
+  </si>
+  <si>
+    <t>This email is already in use.</t>
+  </si>
+  <si>
+    <t>Cet email est déjà utilisé.</t>
+  </si>
+  <si>
+    <t>To gain access to ZombieSurvivor, please verify your e-mail address.</t>
+  </si>
+  <si>
+    <t>Pour accéder à ZombieSurvivor, veuillez vérifier votre adresse e-mail.</t>
+  </si>
+  <si>
+    <t>日本語</t>
+  </si>
+  <si>
+    <t>Comenzar</t>
+  </si>
+  <si>
+    <t>スタート</t>
+  </si>
+  <si>
+    <t>启动</t>
+  </si>
+  <si>
+    <t>Opciones</t>
+  </si>
+  <si>
+    <t>オプション</t>
+  </si>
+  <si>
+    <t>选项</t>
+  </si>
+  <si>
+    <t>Cerrar sesión</t>
+  </si>
+  <si>
+    <t>ログオフする</t>
+  </si>
+  <si>
+    <t>退出登录</t>
+  </si>
+  <si>
+    <t>Salir</t>
+  </si>
+  <si>
+    <t>終了</t>
+  </si>
+  <si>
+    <t>退出</t>
+  </si>
+  <si>
+    <t>Menú principal</t>
+  </si>
+  <si>
+    <t>メイン メニュー</t>
+  </si>
+  <si>
+    <t>主菜单</t>
+  </si>
+  <si>
+    <t>Validar</t>
+  </si>
+  <si>
+    <t>検証する</t>
+  </si>
+  <si>
+    <t>验证</t>
+  </si>
+  <si>
+    <t>Acceso</t>
+  </si>
+  <si>
+    <t>ログイン</t>
+  </si>
+  <si>
+    <t>登录</t>
+  </si>
+  <si>
+    <t>Inscribirse</t>
+  </si>
+  <si>
+    <t>サインアップ</t>
+  </si>
+  <si>
+    <t>报名</t>
+  </si>
+  <si>
+    <t>Correo electrónico</t>
+  </si>
+  <si>
+    <t>メールアドレス</t>
+  </si>
+  <si>
+    <t>电子邮件</t>
+  </si>
+  <si>
+    <t>Contraseña</t>
+  </si>
+  <si>
+    <t>パスワード</t>
+  </si>
+  <si>
+    <t>密码</t>
+  </si>
+  <si>
+    <t>Para obtener acceso a ZombieSurvivor, verifique su dirección de correo electrónico.</t>
+  </si>
+  <si>
+    <t>ZombieSurvivor にアクセスするには、電子メール アドレスを確認してください。</t>
+  </si>
+  <si>
+    <t>要访问 ZombieSurvivor，请验证您的电子邮件地址。</t>
+  </si>
+  <si>
+    <t>¡Iniciado sesión correctamente!</t>
+  </si>
+  <si>
+    <t>ログインに成功しました！</t>
+  </si>
+  <si>
+    <t>登录成功！</t>
+  </si>
+  <si>
+    <t>El inicio de sesión ha fallado.</t>
+  </si>
+  <si>
+    <t>ログインに失敗しました。</t>
+  </si>
+  <si>
+    <t>登录失败。</t>
+  </si>
+  <si>
+    <t>Cuenta creada!</t>
+  </si>
+  <si>
+    <t>アカウントが作成されました！</t>
+  </si>
+  <si>
+    <t>帐户已创建！</t>
+  </si>
+  <si>
+    <t>No se pudo crear la cuenta.</t>
+  </si>
+  <si>
+    <t>アカウントを作成できませんでした。</t>
+  </si>
+  <si>
+    <t>无法创建帐户。</t>
+  </si>
+  <si>
+    <t>El formato del correo electrónico no era válido.</t>
+  </si>
+  <si>
+    <t>メール形式が無効です。</t>
+  </si>
+  <si>
+    <t>电子邮件格式无效。</t>
+  </si>
+  <si>
+    <t>La contraseña no era válida.</t>
+  </si>
+  <si>
+    <t>パスワードが無効です。</t>
+  </si>
+  <si>
+    <t>密码无效。</t>
+  </si>
+  <si>
+    <t>Este correo electrónico ya está en uso.</t>
+  </si>
+  <si>
+    <t>この電子メールは既に利用されています。</t>
+  </si>
+  <si>
+    <t>此电子邮件已被使用。</t>
+  </si>
+  <si>
+    <t>¡Clave válida!</t>
+  </si>
+  <si>
+    <t>有効なキー!</t>
+  </si>
+  <si>
+    <t>有效密钥！</t>
+  </si>
+  <si>
+    <t>¡Tecla inválida!</t>
+  </si>
+  <si>
+    <t>無効キー！</t>
+  </si>
+  <si>
+    <t>无效的密钥！</t>
+  </si>
+  <si>
+    <t>Ola</t>
+  </si>
+  <si>
+    <t>波</t>
+  </si>
+  <si>
+    <t>海浪</t>
+  </si>
+  <si>
+    <t>Retraso de esquivar:</t>
+  </si>
+  <si>
+    <t>回避遅延:</t>
+  </si>
+  <si>
+    <t>闪避延迟</t>
+  </si>
+  <si>
+    <t>sonido principal</t>
+  </si>
+  <si>
+    <t>メインサウンド</t>
+  </si>
+  <si>
+    <t>主音</t>
+  </si>
+  <si>
+    <t>Música</t>
+  </si>
+  <si>
+    <t>音楽</t>
+  </si>
+  <si>
+    <t>音乐</t>
+  </si>
+  <si>
+    <t>视效</t>
+  </si>
+  <si>
+    <t>オーディオ</t>
+  </si>
+  <si>
+    <t>声音的</t>
+  </si>
+  <si>
+    <t>Idioma</t>
+  </si>
+  <si>
+    <t>言語</t>
+  </si>
+  <si>
+    <t>语言</t>
+  </si>
+  <si>
+    <t>Código promocional</t>
+  </si>
+  <si>
+    <t>プロモーションコード</t>
+  </si>
+  <si>
+    <t>促销代码</t>
+  </si>
+  <si>
+    <t>球员数据</t>
+  </si>
+  <si>
+    <t>選手の統計</t>
+  </si>
+  <si>
+    <t>Estadísticas del jugador</t>
+  </si>
+  <si>
+    <t>Invencibilidad:</t>
+  </si>
+  <si>
+    <t>无敌：</t>
+  </si>
+  <si>
+    <t>無敵:</t>
+  </si>
+  <si>
+    <t>Velocidad de movimiento:</t>
+  </si>
+  <si>
+    <t>移动速度：</t>
+  </si>
+  <si>
+    <t>移動速度：</t>
+  </si>
+  <si>
+    <t>Velocidad de ataque:</t>
+  </si>
+  <si>
+    <t>攻撃速度：</t>
+  </si>
+  <si>
+    <t>攻击速度：</t>
+  </si>
+  <si>
+    <t>Velocidad del bumerán:</t>
+  </si>
+  <si>
+    <t>ブーメラン速度:</t>
+  </si>
+  <si>
+    <t>回旋镖速度：</t>
+  </si>
+  <si>
+    <t>Distancia del bumerán:</t>
+  </si>
+  <si>
+    <t>ブーメラン距離:</t>
+  </si>
+  <si>
+    <t>回旋镖距离：</t>
+  </si>
+  <si>
+    <t>简体中文</t>
+  </si>
+  <si>
+    <t>Español</t>
   </si>
 </sst>
 </file>
@@ -1223,10 +1556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1239,7 +1572,7 @@
     <col min="7" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1252,10 +1585,17 @@
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E1" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -1268,10 +1608,17 @@
       <c r="D2" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E2" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
@@ -1284,26 +1631,40 @@
       <c r="D3" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E3" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
@@ -1316,10 +1677,17 @@
       <c r="D5" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E5" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
@@ -1332,10 +1700,17 @@
       <c r="D6" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E6" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
@@ -1348,10 +1723,17 @@
       <c r="D7" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E7" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>61</v>
       </c>
@@ -1364,10 +1746,17 @@
       <c r="D8" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E8" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>63</v>
       </c>
@@ -1380,10 +1769,17 @@
       <c r="D9" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E9" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>69</v>
       </c>
@@ -1396,10 +1792,17 @@
       <c r="D10" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E10" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>72</v>
       </c>
@@ -1412,10 +1815,17 @@
       <c r="D11" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-    </row>
-    <row r="12" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="E11" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>76</v>
       </c>
@@ -1423,333 +1833,549 @@
         <v>77</v>
       </c>
       <c r="C12" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="C20" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-    </row>
-    <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-    </row>
-    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
+      <c r="B21" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="B18" s="4" t="s">
+      <c r="D21" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
+      <c r="E21" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B22" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C22" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D22" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
+      <c r="E22" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B23" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C23" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D23" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E23" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B26" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C29" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D29" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
+      <c r="E29" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B30" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C30" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D30" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="4" t="s">
+      <c r="E30" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B31" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C31" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D31" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="s">
+      <c r="E31" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B32" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C32" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D32" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="4" t="s">
+      <c r="E32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B33" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C33" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D33" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="4" t="s">
+      <c r="E33" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B34" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C34" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D34" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
+      <c r="E34" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>198</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
pivot: priority change - UNFINISHED
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/tsv_UI_Defaults.xlsx
+++ b/Assets/StreamingAssets/tsv_UI_Defaults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Unity Project\metho_misession_MarcSeb\Assets\StreamingAssets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6352DA21-88EE-43F1-B0E2-8DA84E512FE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C0C498E7-C8C6-46B6-842C-39D1174D00AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tsv_UI_Defaults" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="240">
   <si>
     <t>Notes</t>
   </si>
@@ -334,33 +334,18 @@
     <t>Déconnexion</t>
   </si>
   <si>
-    <t>tmp invalid email format</t>
-  </si>
-  <si>
-    <t>tmp invalid password</t>
-  </si>
-  <si>
     <t>The email format was invalid.</t>
   </si>
   <si>
     <t>Le format d'email utilisé est invalide.</t>
   </si>
   <si>
-    <t>Le mot de passe utilisé est invalide.</t>
-  </si>
-  <si>
-    <t>The password was invalid.</t>
-  </si>
-  <si>
     <t>Échec de la connexion.</t>
   </si>
   <si>
     <t>Login has failed.</t>
   </si>
   <si>
-    <t>tmp email already used</t>
-  </si>
-  <si>
     <t>This email is already in use.</t>
   </si>
   <si>
@@ -520,15 +505,6 @@
     <t>电子邮件格式无效。</t>
   </si>
   <si>
-    <t>La contraseña no era válida.</t>
-  </si>
-  <si>
-    <t>パスワードが無効です。</t>
-  </si>
-  <si>
-    <t>密码无效。</t>
-  </si>
-  <si>
     <t>Este correo electrónico ya está en uso.</t>
   </si>
   <si>
@@ -677,6 +653,93 @@
   </si>
   <si>
     <t>Español</t>
+  </si>
+  <si>
+    <t>error password length</t>
+  </si>
+  <si>
+    <t>error email already in used</t>
+  </si>
+  <si>
+    <t>error password number</t>
+  </si>
+  <si>
+    <t>error email format</t>
+  </si>
+  <si>
+    <t>error wrong combination</t>
+  </si>
+  <si>
+    <t>UI Shop</t>
+  </si>
+  <si>
+    <t>tmp shop</t>
+  </si>
+  <si>
+    <t>Shop</t>
+  </si>
+  <si>
+    <t>Boutique</t>
+  </si>
+  <si>
+    <t>The email and/or the password is invalid.</t>
+  </si>
+  <si>
+    <t>The password is too short.</t>
+  </si>
+  <si>
+    <t>UI signup feedback</t>
+  </si>
+  <si>
+    <t>tmp items</t>
+  </si>
+  <si>
+    <t>Items</t>
+  </si>
+  <si>
+    <t>L'email et/ou le mot de passe est invalide.</t>
+  </si>
+  <si>
+    <t>Le mot de passe est trop court.</t>
+  </si>
+  <si>
+    <t>メールまたはパスワードが無効です。</t>
+  </si>
+  <si>
+    <t>电子邮件和/或密码无效。</t>
+  </si>
+  <si>
+    <t>El correo electrónico y/o la contraseña no son válidos.</t>
+  </si>
+  <si>
+    <t>La contraseña es demasiado corta.</t>
+  </si>
+  <si>
+    <t>パスワードが短すぎます。</t>
+  </si>
+  <si>
+    <t>密码太短。</t>
+  </si>
+  <si>
+    <t>店</t>
+  </si>
+  <si>
+    <t>店铺</t>
+  </si>
+  <si>
+    <t>Comercio</t>
+  </si>
+  <si>
+    <t>Elementos</t>
+  </si>
+  <si>
+    <t>项目</t>
+  </si>
+  <si>
+    <t>アイテム</t>
+  </si>
+  <si>
+    <t>TBD</t>
   </si>
 </sst>
 </file>
@@ -819,7 +882,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1008,6 +1071,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1187,7 +1256,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1199,6 +1268,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1556,10 +1628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1586,13 +1658,13 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -1609,13 +1681,13 @@
         <v>54</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -1632,13 +1704,13 @@
         <v>53</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1655,13 +1727,13 @@
         <v>103</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -1678,13 +1750,13 @@
         <v>52</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1701,13 +1773,13 @@
         <v>51</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -1724,13 +1796,13 @@
         <v>60</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -1747,13 +1819,13 @@
         <v>66</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -1770,13 +1842,13 @@
         <v>67</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1793,13 +1865,13 @@
         <v>71</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -1816,13 +1888,13 @@
         <v>75</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
@@ -1833,19 +1905,19 @@
         <v>77</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1862,13 +1934,13 @@
         <v>87</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1879,19 +1951,19 @@
         <v>88</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1908,13 +1980,13 @@
         <v>97</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -1931,243 +2003,243 @@
         <v>99</v>
       </c>
       <c r="E16" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="G18" s="4" t="s">
         <v>160</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>112</v>
+        <v>215</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>113</v>
+        <v>220</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>114</v>
+        <v>225</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>169</v>
+        <v>229</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>170</v>
+        <v>227</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>171</v>
+        <v>228</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B22" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C22" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D22" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="E20" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="E22" s="4" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>14</v>
+        <v>80</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>39</v>
+        <v>81</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>40</v>
+        <v>82</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>201</v>
+        <v>167</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>200</v>
+        <v>168</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>199</v>
+        <v>169</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>202</v>
+        <v>170</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>204</v>
+        <v>171</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>203</v>
+        <v>172</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2175,22 +2247,22 @@
         <v>9</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2198,22 +2270,22 @@
         <v>9</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2221,68 +2293,68 @@
         <v>9</v>
       </c>
       <c r="B29" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C31" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D31" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E29" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>28</v>
-      </c>
       <c r="E31" s="4" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
@@ -2290,92 +2362,211 @@
         <v>22</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>50</v>
+        <v>176</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>50</v>
+        <v>177</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>49</v>
+        <v>179</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B35" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B36" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C36" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="D36" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E34" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="G34" s="4" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A35" s="4" t="s">
+      <c r="E36" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B37" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C37" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="D37" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="E35" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="G35" s="4" t="s">
-        <v>198</v>
-      </c>
+      <c r="E37" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix: debug a null reference due to a TSV file break line
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/tsv_UI_Defaults.xlsx
+++ b/Assets/StreamingAssets/tsv_UI_Defaults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Unity Project\metho_misession_MarcSeb\Assets\StreamingAssets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C0C498E7-C8C6-46B6-842C-39D1174D00AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4E215EF7-1ACB-4704-A77E-96F2F3B99314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1256,7 +1256,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1271,6 +1271,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1630,8 +1633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2542,31 +2545,31 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="4"/>
-      <c r="B40" s="4"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
+      <c r="A40" s="6"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="4"/>
-      <c r="B41" s="4"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="4"/>
+      <c r="A41" s="6"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="4"/>
-      <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="4"/>
-      <c r="F42" s="4"/>
-      <c r="G42" s="4"/>
+      <c r="A42" s="6"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: create logic basis for COR validation
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/tsv_UI_Defaults.xlsx
+++ b/Assets/StreamingAssets/tsv_UI_Defaults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Unity Project\metho_misession_MarcSeb\Assets\StreamingAssets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4E215EF7-1ACB-4704-A77E-96F2F3B99314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C763D2E-D50D-4E0B-A3AA-6C46FF7D7A87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="246">
   <si>
     <t>Notes</t>
   </si>
@@ -658,9 +658,6 @@
     <t>error password length</t>
   </si>
   <si>
-    <t>error email already in used</t>
-  </si>
-  <si>
     <t>error password number</t>
   </si>
   <si>
@@ -740,6 +737,27 @@
   </si>
   <si>
     <t>TBD</t>
+  </si>
+  <si>
+    <t>error email already in use</t>
+  </si>
+  <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>TEST_DO NOT LOCALIZE</t>
+  </si>
+  <si>
+    <t>TEST动</t>
+  </si>
+  <si>
+    <t>TEST óñ</t>
+  </si>
+  <si>
+    <t>TESTéà</t>
+  </si>
+  <si>
+    <t>TEST日本かゲ</t>
   </si>
 </sst>
 </file>
@@ -1256,7 +1274,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1271,9 +1289,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1631,10 +1646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1670,27 +1685,27 @@
         <v>209</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>8</v>
+        <v>241</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>6</v>
+        <v>240</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>55</v>
+        <v>240</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>54</v>
+        <v>244</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>113</v>
+        <v>243</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>114</v>
+        <v>245</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>115</v>
+        <v>242</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -1698,68 +1713,68 @@
         <v>8</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>101</v>
+        <v>5</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>102</v>
+        <v>53</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>103</v>
+        <v>53</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>4</v>
+        <v>101</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>56</v>
+        <v>102</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>52</v>
+        <v>103</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1767,22 +1782,22 @@
         <v>8</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -1790,160 +1805,160 @@
         <v>8</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>58</v>
+        <v>7</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B10" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C10" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E10" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F10" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G10" s="4" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+    <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B11" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D11" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F11" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G11" s="4" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B12" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C12" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D12" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E12" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F12" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G12" s="4" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+    <row r="13" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B13" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C13" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D13" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E13" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F13" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G13" s="4" t="s">
         <v>145</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1951,206 +1966,206 @@
         <v>85</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>94</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C17" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D17" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E17" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F17" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="G17" s="4" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="C17" s="4" t="s">
+    <row r="18" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D18" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E18" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F18" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="G18" s="4" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>85</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>220</v>
+        <v>104</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>225</v>
+        <v>105</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>229</v>
+        <v>158</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>227</v>
+        <v>159</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>85</v>
       </c>
       <c r="B20" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>221</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>226</v>
-      </c>
-      <c r="E20" s="4" t="s">
+      <c r="C21" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="F21" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="G21" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="G20" s="4" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="5" t="s">
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>166</v>
+      <c r="B22" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2158,114 +2173,114 @@
         <v>79</v>
       </c>
       <c r="B23" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C24" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D24" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E24" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="F24" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="G23" s="4" t="s">
+      <c r="G24" s="4" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B25" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C25" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D25" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E25" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="F24" s="4" t="s">
+      <c r="F25" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="G24" s="4" t="s">
+      <c r="G25" s="4" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
+    <row r="26" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B26" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C26" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D26" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E26" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="F25" s="4" t="s">
+      <c r="F26" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="G25" s="4" t="s">
+      <c r="G26" s="4" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2273,22 +2288,22 @@
         <v>9</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2296,22 +2311,22 @@
         <v>9</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2319,22 +2334,22 @@
         <v>9</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2342,45 +2357,45 @@
         <v>9</v>
       </c>
       <c r="B31" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C32" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D32" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="E32" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="F31" s="4" t="s">
+      <c r="F32" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="G31" s="4" t="s">
+      <c r="G32" s="4" t="s">
         <v>175</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -2388,22 +2403,22 @@
         <v>22</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -2411,45 +2426,45 @@
         <v>22</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>50</v>
+        <v>179</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>50</v>
+        <v>180</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>183</v>
+        <v>50</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
@@ -2457,119 +2472,115 @@
         <v>30</v>
       </c>
       <c r="B36" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B37" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C37" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="D37" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E36" s="4" t="s">
+      <c r="E37" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="F36" s="4" t="s">
+      <c r="F37" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="G36" s="4" t="s">
+      <c r="G37" s="4" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A37" s="4" t="s">
+    <row r="38" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B38" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C38" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="D38" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="E38" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="F37" s="4" t="s">
+      <c r="F38" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="G37" s="4" t="s">
+      <c r="G38" s="4" t="s">
         <v>190</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>217</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>219</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>233</v>
-      </c>
-      <c r="G38" s="4" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B39" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="C39" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="C40" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="C39" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="E39" s="4" t="s">
+      <c r="D40" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="G40" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="F39" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="G39" s="4" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="6"/>
-      <c r="B40" s="6"/>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
-      <c r="G40" s="6"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="6"/>
-      <c r="B41" s="6"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
-      <c r="G41" s="6"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="6"/>
-      <c r="B42" s="6"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
-      <c r="G42" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: add last localization to TSV file
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/tsv_UI_Defaults.xlsx
+++ b/Assets/StreamingAssets/tsv_UI_Defaults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Unity Project\metho_misession_MarcSeb\Assets\StreamingAssets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C763D2E-D50D-4E0B-A3AA-6C46FF7D7A87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CA0F0E83-6CF1-4E4A-93A8-EBFA61D42496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="251">
   <si>
     <t>Notes</t>
   </si>
@@ -736,9 +736,6 @@
     <t>アイテム</t>
   </si>
   <si>
-    <t>TBD</t>
-  </si>
-  <si>
     <t>error email already in use</t>
   </si>
   <si>
@@ -758,6 +755,24 @@
   </si>
   <si>
     <t>TEST日本かゲ</t>
+  </si>
+  <si>
+    <t>The password must have at least one number.</t>
+  </si>
+  <si>
+    <t>Le mot de passe doit contenir au moins un numéro.</t>
+  </si>
+  <si>
+    <t>La contraseña debe tener al menos un número.</t>
+  </si>
+  <si>
+    <t>密码必须至少有一个数字。</t>
+  </si>
+  <si>
+    <t>パスワードには少なくとも 1 つの数字が必要です。</t>
+  </si>
+  <si>
+    <t>UI Login/Signup feedback</t>
   </si>
 </sst>
 </file>
@@ -1094,7 +1109,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1648,8 +1663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1687,25 +1702,25 @@
     </row>
     <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>241</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>243</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -2058,7 +2073,7 @@
         <v>221</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>108</v>
@@ -2078,7 +2093,7 @@
     </row>
     <row r="19" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>85</v>
+        <v>250</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>213</v>
@@ -2101,7 +2116,7 @@
     </row>
     <row r="20" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>85</v>
+        <v>250</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>214</v>
@@ -2124,7 +2139,7 @@
     </row>
     <row r="21" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>211</v>
@@ -2145,27 +2160,27 @@
         <v>231</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>212</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>238</v>
+        <v>246</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>238</v>
+        <v>247</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>238</v>
+        <v>249</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>238</v>
+        <v>248</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
feat: add practice ring to practice scene
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/tsv_UI_Defaults.xlsx
+++ b/Assets/StreamingAssets/tsv_UI_Defaults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Unity Project\metho_misession_MarcSeb\Assets\StreamingAssets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CA0F0E83-6CF1-4E4A-93A8-EBFA61D42496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D7FB7B3D-859B-4B59-ACE4-ECD80578FC04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tsv_UI_Defaults" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="264">
   <si>
     <t>Notes</t>
   </si>
@@ -773,6 +773,45 @@
   </si>
   <si>
     <t>UI Login/Signup feedback</t>
+  </si>
+  <si>
+    <t>UI Scene name</t>
+  </si>
+  <si>
+    <t>tmp practice room</t>
+  </si>
+  <si>
+    <t>Practice Room</t>
+  </si>
+  <si>
+    <t>練習室</t>
+  </si>
+  <si>
+    <t>练习室</t>
+  </si>
+  <si>
+    <t>Salle de Test</t>
+  </si>
+  <si>
+    <t>Sala de Prueba</t>
+  </si>
+  <si>
+    <t>btn play offline</t>
+  </si>
+  <si>
+    <t>Play offline</t>
+  </si>
+  <si>
+    <t>オフライン</t>
+  </si>
+  <si>
+    <t>Juego local</t>
+  </si>
+  <si>
+    <t>Jouer localement</t>
+  </si>
+  <si>
+    <t>本地播放</t>
   </si>
 </sst>
 </file>
@@ -1661,10 +1700,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2597,6 +2636,52 @@
         <v>236</v>
       </c>
     </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>263</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
feat: create localization for tutorial texts
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/tsv_UI_Defaults.xlsx
+++ b/Assets/StreamingAssets/tsv_UI_Defaults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Unity Project\metho_misession_MarcSeb\Assets\StreamingAssets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D7FB7B3D-859B-4B59-ACE4-ECD80578FC04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{835FCED3-79D2-4140-AB26-A98387C9C56F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="301">
   <si>
     <t>Notes</t>
   </si>
@@ -812,6 +812,117 @@
   </si>
   <si>
     <t>本地播放</t>
+  </si>
+  <si>
+    <t>Tutorial text</t>
+  </si>
+  <si>
+    <t>tutorial wave</t>
+  </si>
+  <si>
+    <t>tutorial skills</t>
+  </si>
+  <si>
+    <t>tutorial currency</t>
+  </si>
+  <si>
+    <t>tutorial chest</t>
+  </si>
+  <si>
+    <t>tutorial potion</t>
+  </si>
+  <si>
+    <t>tutorial boss portal</t>
+  </si>
+  <si>
+    <t>Information on the current wave is located here: timer, name, etc.</t>
+  </si>
+  <si>
+    <t>Your skills. Some can be used more often than others.</t>
+  </si>
+  <si>
+    <t>Your currency. Use it to open chests!</t>
+  </si>
+  <si>
+    <t>A bonus chest. Open it to grow more powerful!</t>
+  </si>
+  <si>
+    <t>One potion a day keeps the doctor away.</t>
+  </si>
+  <si>
+    <t>La información sobre la ola actual se encuentra aquí: temporizador, nombre, etc.</t>
+  </si>
+  <si>
+    <t>当前波形的信息位于此处：计时器、名称等。</t>
+  </si>
+  <si>
+    <t>現在のウェーブに関する情報はここにあります: タイマー、名前など。</t>
+  </si>
+  <si>
+    <t>你的技能。有些可以比其他更频繁地使用。</t>
+  </si>
+  <si>
+    <t>あなたの技術。他のものより頻繁に使用できるものもあります。</t>
+  </si>
+  <si>
+    <t>Tus habilidades. Algunos se pueden usar con más frecuencia que otros.</t>
+  </si>
+  <si>
+    <t>Tu moneda. ¡Úsalo para abrir cofres!</t>
+  </si>
+  <si>
+    <t>あなたの通貨。それを使って宝箱を開けよう！</t>
+  </si>
+  <si>
+    <t>你的货币。用它来打开箱子！</t>
+  </si>
+  <si>
+    <t>Un cofre de bonificación. ¡Ábrelo para volverte más poderoso!</t>
+  </si>
+  <si>
+    <t>一个奖金箱子。打开它变得更强大！</t>
+  </si>
+  <si>
+    <t>ボーナスチェスト。それを開いて、より強力に成長してください！</t>
+  </si>
+  <si>
+    <t>一天一剂，医生远离我。</t>
+  </si>
+  <si>
+    <t>1日1錠で医者いらず。</t>
+  </si>
+  <si>
+    <t>Una poción al día mantiene alejado al médico.</t>
+  </si>
+  <si>
+    <t>生成关卡 Boss 的传送门。底部的数字表示打开它并召唤 Boss 所需的货币。</t>
+  </si>
+  <si>
+    <t>レベルのボスを生成するポータル。下部の数字は、それを開いてボスを呼び出すために必要な通貨を示しています。</t>
+  </si>
+  <si>
+    <t>Un portal que genera el jefe del nivel. El número en la parte inferior indica la moneda requerida para abrirlo y llamar al jefe.</t>
+  </si>
+  <si>
+    <t>De l'information sur la vague en cours est affichée ici: temps, nom, etc.</t>
+  </si>
+  <si>
+    <t>Vos aptitudes. Certaines peuvent être utilisées plus fréquemment que d'autres.</t>
+  </si>
+  <si>
+    <t>Votre monnaie. Utilisez-la pour ouvrir des coffres!</t>
+  </si>
+  <si>
+    <t>Un coffre bonus. Ouvrez-le pour devenir plus puissant!</t>
+  </si>
+  <si>
+    <t>Une potion par jour garde le médecin au loin!</t>
+  </si>
+  <si>
+    <t>Un portail qui fait apparaître le boss du niveau. Le nombre au bas indique la monnaie nécessaire pour ouvrir le portail et invoquer le boss.</t>
+  </si>
+  <si>
+    <t>A portal that spawns the level's boss.\nThe number at the bottom indicates the required currency to open it and call forth the boss.</t>
   </si>
 </sst>
 </file>
@@ -1700,10 +1811,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2682,6 +2793,144 @@
         <v>263</v>
       </c>
     </row>
+    <row r="43" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A44" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A45" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A46" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A47" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A48" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>291</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
feat: decouple localization to use a scene based one when appropriate
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/tsv_UI_Defaults.xlsx
+++ b/Assets/StreamingAssets/tsv_UI_Defaults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Unity Project\metho_misession_MarcSeb\Assets\StreamingAssets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{835FCED3-79D2-4140-AB26-A98387C9C56F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6A9D2990-EAA3-46E7-9311-E2E266840A68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="264">
   <si>
     <t>Notes</t>
   </si>
@@ -812,117 +812,6 @@
   </si>
   <si>
     <t>本地播放</t>
-  </si>
-  <si>
-    <t>Tutorial text</t>
-  </si>
-  <si>
-    <t>tutorial wave</t>
-  </si>
-  <si>
-    <t>tutorial skills</t>
-  </si>
-  <si>
-    <t>tutorial currency</t>
-  </si>
-  <si>
-    <t>tutorial chest</t>
-  </si>
-  <si>
-    <t>tutorial potion</t>
-  </si>
-  <si>
-    <t>tutorial boss portal</t>
-  </si>
-  <si>
-    <t>Information on the current wave is located here: timer, name, etc.</t>
-  </si>
-  <si>
-    <t>Your skills. Some can be used more often than others.</t>
-  </si>
-  <si>
-    <t>Your currency. Use it to open chests!</t>
-  </si>
-  <si>
-    <t>A bonus chest. Open it to grow more powerful!</t>
-  </si>
-  <si>
-    <t>One potion a day keeps the doctor away.</t>
-  </si>
-  <si>
-    <t>La información sobre la ola actual se encuentra aquí: temporizador, nombre, etc.</t>
-  </si>
-  <si>
-    <t>当前波形的信息位于此处：计时器、名称等。</t>
-  </si>
-  <si>
-    <t>現在のウェーブに関する情報はここにあります: タイマー、名前など。</t>
-  </si>
-  <si>
-    <t>你的技能。有些可以比其他更频繁地使用。</t>
-  </si>
-  <si>
-    <t>あなたの技術。他のものより頻繁に使用できるものもあります。</t>
-  </si>
-  <si>
-    <t>Tus habilidades. Algunos se pueden usar con más frecuencia que otros.</t>
-  </si>
-  <si>
-    <t>Tu moneda. ¡Úsalo para abrir cofres!</t>
-  </si>
-  <si>
-    <t>あなたの通貨。それを使って宝箱を開けよう！</t>
-  </si>
-  <si>
-    <t>你的货币。用它来打开箱子！</t>
-  </si>
-  <si>
-    <t>Un cofre de bonificación. ¡Ábrelo para volverte más poderoso!</t>
-  </si>
-  <si>
-    <t>一个奖金箱子。打开它变得更强大！</t>
-  </si>
-  <si>
-    <t>ボーナスチェスト。それを開いて、より強力に成長してください！</t>
-  </si>
-  <si>
-    <t>一天一剂，医生远离我。</t>
-  </si>
-  <si>
-    <t>1日1錠で医者いらず。</t>
-  </si>
-  <si>
-    <t>Una poción al día mantiene alejado al médico.</t>
-  </si>
-  <si>
-    <t>生成关卡 Boss 的传送门。底部的数字表示打开它并召唤 Boss 所需的货币。</t>
-  </si>
-  <si>
-    <t>レベルのボスを生成するポータル。下部の数字は、それを開いてボスを呼び出すために必要な通貨を示しています。</t>
-  </si>
-  <si>
-    <t>Un portal que genera el jefe del nivel. El número en la parte inferior indica la moneda requerida para abrirlo y llamar al jefe.</t>
-  </si>
-  <si>
-    <t>De l'information sur la vague en cours est affichée ici: temps, nom, etc.</t>
-  </si>
-  <si>
-    <t>Vos aptitudes. Certaines peuvent être utilisées plus fréquemment que d'autres.</t>
-  </si>
-  <si>
-    <t>Votre monnaie. Utilisez-la pour ouvrir des coffres!</t>
-  </si>
-  <si>
-    <t>Un coffre bonus. Ouvrez-le pour devenir plus puissant!</t>
-  </si>
-  <si>
-    <t>Une potion par jour garde le médecin au loin!</t>
-  </si>
-  <si>
-    <t>Un portail qui fait apparaître le boss du niveau. Le nombre au bas indique la monnaie nécessaire pour ouvrir le portail et invoquer le boss.</t>
-  </si>
-  <si>
-    <t>A portal that spawns the level's boss.\nThe number at the bottom indicates the required currency to open it and call forth the boss.</t>
   </si>
 </sst>
 </file>
@@ -1811,10 +1700,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2793,144 +2682,6 @@
         <v>263</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A43" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>294</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="F43" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="G43" s="4" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A44" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>281</v>
-      </c>
-      <c r="F44" s="4" t="s">
-        <v>280</v>
-      </c>
-      <c r="G44" s="4" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A45" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>273</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>296</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>282</v>
-      </c>
-      <c r="F45" s="4" t="s">
-        <v>283</v>
-      </c>
-      <c r="G45" s="4" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A46" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>268</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>274</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>297</v>
-      </c>
-      <c r="E46" s="4" t="s">
-        <v>285</v>
-      </c>
-      <c r="F46" s="4" t="s">
-        <v>287</v>
-      </c>
-      <c r="G46" s="4" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A47" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>269</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>275</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>298</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>290</v>
-      </c>
-      <c r="F47" s="4" t="s">
-        <v>289</v>
-      </c>
-      <c r="G47" s="4" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A48" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>270</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>300</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>299</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>293</v>
-      </c>
-      <c r="F48" s="4" t="s">
-        <v>292</v>
-      </c>
-      <c r="G48" s="4" t="s">
-        <v>291</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
feat: create base setup for shopview
Mockups are presents to facilitate the logic implementation.
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/tsv_UI_Defaults.xlsx
+++ b/Assets/StreamingAssets/tsv_UI_Defaults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Unity Project\metho_misession_MarcSeb\Assets\StreamingAssets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6A9D2990-EAA3-46E7-9311-E2E266840A68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8E21CD83-FA60-4174-B9AD-FDC7B96BC69A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="270">
   <si>
     <t>Notes</t>
   </si>
@@ -121,48 +121,12 @@
     <t>tmp tab language</t>
   </si>
   <si>
-    <t>Attack speed:</t>
-  </si>
-  <si>
-    <t>Boomerang speed:</t>
-  </si>
-  <si>
-    <t>Boomerang distance:</t>
-  </si>
-  <si>
-    <t>Dodge delay:</t>
-  </si>
-  <si>
-    <t>Move speed:</t>
-  </si>
-  <si>
-    <t>Invincibility:</t>
-  </si>
-  <si>
     <t>Player stats</t>
   </si>
   <si>
     <t>Statistiques joueur</t>
   </si>
   <si>
-    <t>Invincibilité:</t>
-  </si>
-  <si>
-    <t>Vitesse de déplacement:</t>
-  </si>
-  <si>
-    <t>Vitesse d'attaque:</t>
-  </si>
-  <si>
-    <t>Vitesse du boomerang:</t>
-  </si>
-  <si>
-    <t>Distance du boomerang:</t>
-  </si>
-  <si>
-    <t>Délais d'esquive:</t>
-  </si>
-  <si>
     <t>Langage</t>
   </si>
   <si>
@@ -541,12 +505,6 @@
     <t>海浪</t>
   </si>
   <si>
-    <t>Retraso de esquivar:</t>
-  </si>
-  <si>
-    <t>回避遅延:</t>
-  </si>
-  <si>
     <t>闪避延迟</t>
   </si>
   <si>
@@ -604,51 +562,6 @@
     <t>Estadísticas del jugador</t>
   </si>
   <si>
-    <t>Invencibilidad:</t>
-  </si>
-  <si>
-    <t>无敌：</t>
-  </si>
-  <si>
-    <t>無敵:</t>
-  </si>
-  <si>
-    <t>Velocidad de movimiento:</t>
-  </si>
-  <si>
-    <t>移动速度：</t>
-  </si>
-  <si>
-    <t>移動速度：</t>
-  </si>
-  <si>
-    <t>Velocidad de ataque:</t>
-  </si>
-  <si>
-    <t>攻撃速度：</t>
-  </si>
-  <si>
-    <t>攻击速度：</t>
-  </si>
-  <si>
-    <t>Velocidad del bumerán:</t>
-  </si>
-  <si>
-    <t>ブーメラン速度:</t>
-  </si>
-  <si>
-    <t>回旋镖速度：</t>
-  </si>
-  <si>
-    <t>Distancia del bumerán:</t>
-  </si>
-  <si>
-    <t>ブーメラン距離:</t>
-  </si>
-  <si>
-    <t>回旋镖距离：</t>
-  </si>
-  <si>
     <t>简体中文</t>
   </si>
   <si>
@@ -812,6 +725,111 @@
   </si>
   <si>
     <t>本地播放</t>
+  </si>
+  <si>
+    <t>btn shop convert currency</t>
+  </si>
+  <si>
+    <t>Convert Currency</t>
+  </si>
+  <si>
+    <t>Convertir la monnaie</t>
+  </si>
+  <si>
+    <t>Convertir moneda</t>
+  </si>
+  <si>
+    <t>通貨を換算</t>
+  </si>
+  <si>
+    <t>转换货币</t>
+  </si>
+  <si>
+    <t>Vitesse du boomerang</t>
+  </si>
+  <si>
+    <t>Vitesse d'attaque</t>
+  </si>
+  <si>
+    <t>Vitesse de déplacement</t>
+  </si>
+  <si>
+    <t>Invincibilité</t>
+  </si>
+  <si>
+    <t>Distance du boomerang</t>
+  </si>
+  <si>
+    <t>Délais d'esquive</t>
+  </si>
+  <si>
+    <t>Retraso de esquivar</t>
+  </si>
+  <si>
+    <t>Distancia del bumerán</t>
+  </si>
+  <si>
+    <t>Velocidad del bumerán</t>
+  </si>
+  <si>
+    <t>Velocidad de movimiento</t>
+  </si>
+  <si>
+    <t>Invencibilidad</t>
+  </si>
+  <si>
+    <t>無敵</t>
+  </si>
+  <si>
+    <t>无敌</t>
+  </si>
+  <si>
+    <t>攻击速度</t>
+  </si>
+  <si>
+    <t>移动速度</t>
+  </si>
+  <si>
+    <t>回旋镖距离</t>
+  </si>
+  <si>
+    <t>回旋镖速度</t>
+  </si>
+  <si>
+    <t>ブーメラン速度</t>
+  </si>
+  <si>
+    <t>攻撃速度</t>
+  </si>
+  <si>
+    <t>移動速度</t>
+  </si>
+  <si>
+    <t>ブーメラン距離</t>
+  </si>
+  <si>
+    <t>回避遅延</t>
+  </si>
+  <si>
+    <t>Velocidad de ataque</t>
+  </si>
+  <si>
+    <t>Boomerang speed</t>
+  </si>
+  <si>
+    <t>Attack speed</t>
+  </si>
+  <si>
+    <t>Move speed</t>
+  </si>
+  <si>
+    <t>Invincibility</t>
+  </si>
+  <si>
+    <t>Boomerang distance</t>
+  </si>
+  <si>
+    <t>Dodge delay</t>
   </si>
 </sst>
 </file>
@@ -1700,10 +1718,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1730,36 +1748,36 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>210</v>
+        <v>181</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>209</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>240</v>
+        <v>211</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>239</v>
+        <v>210</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>239</v>
+        <v>210</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>243</v>
+        <v>214</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>242</v>
+        <v>213</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>241</v>
+        <v>212</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -1770,19 +1788,19 @@
         <v>6</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -1793,19 +1811,19 @@
         <v>5</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1813,22 +1831,22 @@
         <v>8</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1839,19 +1857,19 @@
         <v>4</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -1862,19 +1880,19 @@
         <v>7</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -1882,390 +1900,390 @@
         <v>8</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>221</v>
+        <v>192</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>238</v>
+        <v>209</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>250</v>
+        <v>221</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>213</v>
+        <v>184</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>250</v>
+        <v>221</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>214</v>
+        <v>185</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>219</v>
+        <v>190</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>224</v>
+        <v>195</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>228</v>
+        <v>199</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>226</v>
+        <v>197</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>227</v>
+        <v>198</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>211</v>
+        <v>182</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>220</v>
+        <v>191</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>225</v>
+        <v>196</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>229</v>
+        <v>200</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>230</v>
+        <v>201</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>231</v>
+        <v>202</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>212</v>
+        <v>183</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>245</v>
+        <v>216</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>246</v>
+        <v>217</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>247</v>
+        <v>218</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>249</v>
+        <v>220</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>248</v>
+        <v>219</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -2282,13 +2300,13 @@
         <v>12</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2299,19 +2317,19 @@
         <v>14</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -2322,19 +2340,19 @@
         <v>16</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>38</v>
+        <v>267</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>41</v>
+        <v>244</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>194</v>
+        <v>251</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>196</v>
+        <v>252</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>195</v>
+        <v>253</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2345,19 +2363,19 @@
         <v>17</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>37</v>
+        <v>266</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>42</v>
+        <v>243</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>197</v>
+        <v>250</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>199</v>
+        <v>260</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>198</v>
+        <v>255</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2368,19 +2386,19 @@
         <v>18</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>33</v>
+        <v>265</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>43</v>
+        <v>242</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>200</v>
+        <v>263</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>201</v>
+        <v>259</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>202</v>
+        <v>254</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2391,19 +2409,19 @@
         <v>20</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>34</v>
+        <v>264</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>44</v>
+        <v>241</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>203</v>
+        <v>249</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>204</v>
+        <v>258</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>205</v>
+        <v>257</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2414,19 +2432,19 @@
         <v>19</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>35</v>
+        <v>268</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>45</v>
+        <v>245</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>206</v>
+        <v>248</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>207</v>
+        <v>261</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>208</v>
+        <v>256</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2437,19 +2455,19 @@
         <v>21</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>36</v>
+        <v>269</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>46</v>
+        <v>246</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>173</v>
+        <v>247</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>174</v>
+        <v>262</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -2466,13 +2484,13 @@
         <v>29</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -2489,13 +2507,13 @@
         <v>28</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -2506,19 +2524,19 @@
         <v>25</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
@@ -2529,19 +2547,19 @@
         <v>31</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -2552,111 +2570,111 @@
         <v>32</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
-        <v>215</v>
+        <v>186</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>216</v>
+        <v>187</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>217</v>
+        <v>188</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>218</v>
+        <v>189</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>234</v>
+        <v>205</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>232</v>
+        <v>203</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>233</v>
+        <v>204</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
-        <v>215</v>
+        <v>186</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>222</v>
+        <v>193</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>223</v>
+        <v>194</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>223</v>
+        <v>194</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>235</v>
+        <v>206</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>237</v>
+        <v>208</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>236</v>
+        <v>207</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
-        <v>251</v>
+        <v>222</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>252</v>
+        <v>223</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>253</v>
+        <v>224</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>256</v>
+        <v>227</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>257</v>
+        <v>228</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>254</v>
+        <v>225</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>255</v>
+        <v>226</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2664,22 +2682,45 @@
         <v>8</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>258</v>
+        <v>229</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>259</v>
+        <v>230</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>262</v>
+        <v>233</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>261</v>
+        <v>232</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>260</v>
+        <v>231</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>263</v>
+        <v>234</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>240</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add win screen transition
Also debugged missing references in option menu tab buttons
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/tsv_UI_Defaults.xlsx
+++ b/Assets/StreamingAssets/tsv_UI_Defaults.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Unity Project\metho_misession_MarcSeb\Assets\StreamingAssets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8E21CD83-FA60-4174-B9AD-FDC7B96BC69A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A82A3FC-AD30-487E-95E0-F9FF303A32AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="284">
   <si>
     <t>Notes</t>
   </si>
@@ -830,6 +830,48 @@
   </si>
   <si>
     <t>Dodge delay</t>
+  </si>
+  <si>
+    <t>Game won</t>
+  </si>
+  <si>
+    <t>Death</t>
+  </si>
+  <si>
+    <t>tmp game won</t>
+  </si>
+  <si>
+    <t>tmp game lost</t>
+  </si>
+  <si>
+    <t>You died!</t>
+  </si>
+  <si>
+    <t>You survived!</t>
+  </si>
+  <si>
+    <t>Vous avez survécu!</t>
+  </si>
+  <si>
+    <t>Vous êtes mort!</t>
+  </si>
+  <si>
+    <t>¡Moriste!</t>
+  </si>
+  <si>
+    <t>¡Sobreviviste!</t>
+  </si>
+  <si>
+    <t>死にました！</t>
+  </si>
+  <si>
+    <t>生き残った！</t>
+  </si>
+  <si>
+    <t>你活下来了！</t>
+  </si>
+  <si>
+    <t>你死了！</t>
   </si>
 </sst>
 </file>
@@ -1718,10 +1760,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2723,6 +2765,52 @@
         <v>240</v>
       </c>
     </row>
+    <row r="44" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A44" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A45" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fix: redo methods and prefabs that were overloaded after last merge
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/tsv_UI_Defaults.xlsx
+++ b/Assets/StreamingAssets/tsv_UI_Defaults.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Unity Project\metho_misession_MarcSeb\Assets\StreamingAssets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8E21CD83-FA60-4174-B9AD-FDC7B96BC69A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F48C3968-089A-4443-B45D-204B3476958A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="284">
   <si>
     <t>Notes</t>
   </si>
@@ -830,6 +830,48 @@
   </si>
   <si>
     <t>Dodge delay</t>
+  </si>
+  <si>
+    <t>tmp game won</t>
+  </si>
+  <si>
+    <t>Win screen</t>
+  </si>
+  <si>
+    <t>Death screen</t>
+  </si>
+  <si>
+    <t>You died!</t>
+  </si>
+  <si>
+    <t>tmp game lost</t>
+  </si>
+  <si>
+    <t>Vous avez survécu!</t>
+  </si>
+  <si>
+    <t>You survived!</t>
+  </si>
+  <si>
+    <t>死にました！</t>
+  </si>
+  <si>
+    <t>¡Sobreviviste!</t>
+  </si>
+  <si>
+    <t>生き残った！</t>
+  </si>
+  <si>
+    <t>你活下来了！</t>
+  </si>
+  <si>
+    <t>你死了！</t>
+  </si>
+  <si>
+    <t>¡Moriste!</t>
+  </si>
+  <si>
+    <t>Vous avez péri!</t>
   </si>
 </sst>
 </file>
@@ -1718,10 +1760,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2723,6 +2765,52 @@
         <v>240</v>
       </c>
     </row>
+    <row r="44" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A44" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A45" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>281</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
feat: add visual cues to promo code entries
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/tsv_UI_Defaults.xlsx
+++ b/Assets/StreamingAssets/tsv_UI_Defaults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Unity Project\metho_misession_MarcSeb\Assets\StreamingAssets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F48C3968-089A-4443-B45D-204B3476958A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EEAD7C53-23D6-4023-ABCF-36D1AA4691E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="321">
   <si>
     <t>Notes</t>
   </si>
@@ -872,6 +872,117 @@
   </si>
   <si>
     <t>Vous avez péri!</t>
+  </si>
+  <si>
+    <t>UI promo code cue</t>
+  </si>
+  <si>
+    <t>tmp promo perma stat</t>
+  </si>
+  <si>
+    <t>tmp promo temp stat</t>
+  </si>
+  <si>
+    <t>tmp promo big currency</t>
+  </si>
+  <si>
+    <t>tmp promo small currency</t>
+  </si>
+  <si>
+    <t>Big currency otained!</t>
+  </si>
+  <si>
+    <t>Small currency obtained!</t>
+  </si>
+  <si>
+    <t>Petite monnaie obtenue!</t>
+  </si>
+  <si>
+    <t>Grosse monnaie obtenue!</t>
+  </si>
+  <si>
+    <t>Statistique permanente obtenue!</t>
+  </si>
+  <si>
+    <t>Statistique temporaire obtenue!</t>
+  </si>
+  <si>
+    <t>Permanent statistic obtained!</t>
+  </si>
+  <si>
+    <t>Temporary statistic obtained!</t>
+  </si>
+  <si>
+    <t>¡Pequeña moneda obtenida!</t>
+  </si>
+  <si>
+    <t>Gran moneda obtenida!</t>
+  </si>
+  <si>
+    <t>获得大额货币！</t>
+  </si>
+  <si>
+    <t>小货币获得！</t>
+  </si>
+  <si>
+    <t>小さな通貨を手に入れた！</t>
+  </si>
+  <si>
+    <t>大きな通貨を手に入れた！</t>
+  </si>
+  <si>
+    <t>永久統計取得！</t>
+  </si>
+  <si>
+    <t>暫定統計取得！</t>
+  </si>
+  <si>
+    <t>临时统计得到！</t>
+  </si>
+  <si>
+    <t>获得永久统计！</t>
+  </si>
+  <si>
+    <t>¡Estadística permanente obtenida!</t>
+  </si>
+  <si>
+    <t>¡Estadística temporal obtenida!</t>
+  </si>
+  <si>
+    <t>tmp psFullHeal</t>
+  </si>
+  <si>
+    <t>tmp psHealthUp</t>
+  </si>
+  <si>
+    <t>Full heal</t>
+  </si>
+  <si>
+    <t>Health up</t>
+  </si>
+  <si>
+    <t>Soin complet</t>
+  </si>
+  <si>
+    <t>Points de vie additionnels</t>
+  </si>
+  <si>
+    <t>Totalmente curado</t>
+  </si>
+  <si>
+    <t>完全治愈</t>
+  </si>
+  <si>
+    <t>フルヒール</t>
+  </si>
+  <si>
+    <t>ヘルスアップ</t>
+  </si>
+  <si>
+    <t>健康起来</t>
+  </si>
+  <si>
+    <t>Salud arriba</t>
   </si>
 </sst>
 </file>
@@ -1760,10 +1871,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2328,165 +2439,165 @@
         <v>157</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B29" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C29" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D29" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E29" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="F25" s="4" t="s">
+      <c r="F29" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="G25" s="4" t="s">
+      <c r="G29" s="4" t="s">
         <v>160</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A28" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>243</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>260</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>263</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>259</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>264</v>
+        <v>33</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>241</v>
+        <v>34</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>249</v>
+        <v>179</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>258</v>
+        <v>178</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2494,320 +2605,458 @@
         <v>9</v>
       </c>
       <c r="B32" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C36" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D36" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="E36" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="F32" s="4" t="s">
+      <c r="F36" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="G32" s="4" t="s">
+      <c r="G36" s="4" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="G34" s="4" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G35" s="4" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="G36" s="4" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>32</v>
+        <v>309</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>36</v>
+        <v>311</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>35</v>
+        <v>313</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>171</v>
+        <v>315</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>172</v>
+        <v>317</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>173</v>
+        <v>316</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
-        <v>78</v>
+        <v>9</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>79</v>
+        <v>310</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>80</v>
+        <v>312</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>81</v>
+        <v>314</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>174</v>
+        <v>320</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>175</v>
+        <v>318</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>176</v>
+        <v>319</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
-        <v>186</v>
+        <v>22</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>187</v>
+        <v>23</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>188</v>
+        <v>26</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>189</v>
+        <v>29</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>205</v>
+        <v>162</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>203</v>
+        <v>163</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>204</v>
+        <v>164</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
-        <v>186</v>
+        <v>22</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>193</v>
+        <v>24</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>194</v>
+        <v>27</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>194</v>
+        <v>28</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>206</v>
+        <v>165</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>208</v>
+        <v>166</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>207</v>
+        <v>167</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
-        <v>222</v>
+        <v>22</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>223</v>
+        <v>25</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>224</v>
+        <v>38</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>227</v>
+        <v>38</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>228</v>
+        <v>38</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>225</v>
+        <v>38</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>229</v>
+        <v>31</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>230</v>
+        <v>37</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>233</v>
+        <v>37</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>232</v>
+        <v>37</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>231</v>
+        <v>169</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>235</v>
+        <v>32</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>236</v>
+        <v>36</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>237</v>
+        <v>35</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>238</v>
+        <v>171</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>239</v>
+        <v>172</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>240</v>
+        <v>173</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A48" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A49" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="G49" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A50" s="4" t="s">
         <v>271</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B50" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C50" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="D44" s="4" t="s">
+      <c r="D50" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="E44" s="4" t="s">
+      <c r="E50" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="F44" s="4" t="s">
+      <c r="F50" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="G44" s="4" t="s">
+      <c r="G50" s="4" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A45" s="4" t="s">
+    <row r="51" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A51" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B51" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="C51" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="D45" s="4" t="s">
+      <c r="D51" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="E45" s="4" t="s">
+      <c r="E51" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="F45" s="4" t="s">
+      <c r="F51" s="4" t="s">
         <v>277</v>
       </c>
-      <c r="G45" s="4" t="s">
+      <c r="G51" s="4" t="s">
         <v>281</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: add localization for chest and potion bonus pickup
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/tsv_UI_Defaults.xlsx
+++ b/Assets/StreamingAssets/tsv_UI_Defaults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Unity Project\metho_misession_MarcSeb\Assets\StreamingAssets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EEAD7C53-23D6-4023-ABCF-36D1AA4691E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{946F7723-30E1-4C65-932F-B29682D0D715}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="327">
   <si>
     <t>Notes</t>
   </si>
@@ -983,6 +983,24 @@
   </si>
   <si>
     <t>Salud arriba</t>
+  </si>
+  <si>
+    <t>tmp noMoreUpgrades</t>
+  </si>
+  <si>
+    <t>No more upgrades…</t>
+  </si>
+  <si>
+    <t>Aucun bonus restant…</t>
+  </si>
+  <si>
+    <t>没有更多的升级</t>
+  </si>
+  <si>
+    <t>もうアップグレードはありません</t>
+  </si>
+  <si>
+    <t>No más actualizaciones</t>
   </si>
 </sst>
 </file>
@@ -1871,10 +1889,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2761,27 +2779,27 @@
         <v>319</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>23</v>
+        <v>321</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>26</v>
+        <v>322</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>29</v>
+        <v>323</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>162</v>
+        <v>326</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>163</v>
+        <v>325</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>164</v>
+        <v>324</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
@@ -2789,22 +2807,22 @@
         <v>22</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
@@ -2812,45 +2830,45 @@
         <v>22</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>38</v>
+        <v>165</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>38</v>
+        <v>166</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>169</v>
+        <v>38</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
@@ -2858,68 +2876,68 @@
         <v>30</v>
       </c>
       <c r="B43" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B44" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C44" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D43" s="4" t="s">
+      <c r="D44" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E43" s="4" t="s">
+      <c r="E44" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="F43" s="4" t="s">
+      <c r="F44" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="G43" s="4" t="s">
+      <c r="G44" s="4" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A44" s="4" t="s">
+    <row r="45" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A45" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B45" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C45" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="D44" s="4" t="s">
+      <c r="D45" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E44" s="4" t="s">
+      <c r="E45" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="F44" s="4" t="s">
+      <c r="F45" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="G44" s="4" t="s">
+      <c r="G45" s="4" t="s">
         <v>176</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="F45" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="G45" s="4" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
@@ -2927,68 +2945,68 @@
         <v>186</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B48" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="C48" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="D47" s="4" t="s">
+      <c r="D48" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="E47" s="4" t="s">
+      <c r="E48" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="F47" s="4" t="s">
+      <c r="F48" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="G47" s="4" t="s">
+      <c r="G48" s="4" t="s">
         <v>226</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A48" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>233</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="F48" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="G48" s="4" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2996,67 +3014,90 @@
         <v>8</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
-        <v>271</v>
+        <v>8</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>270</v>
+        <v>235</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>276</v>
+        <v>236</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>275</v>
+        <v>237</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>278</v>
+        <v>238</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>279</v>
+        <v>239</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>280</v>
+        <v>240</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="G51" s="4" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A52" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B52" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C52" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="D51" s="4" t="s">
+      <c r="D52" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="E51" s="4" t="s">
+      <c r="E52" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="F51" s="4" t="s">
+      <c r="F52" s="4" t="s">
         <v>277</v>
       </c>
-      <c r="G51" s="4" t="s">
+      <c r="G52" s="4" t="s">
         <v>281</v>
       </c>
     </row>

</xml_diff>